<commit_message>
K Means Cluster Analysis Program
A Node JS program to perform K Means Cluster Analysis using Elbow Method for calculating number of clusters
</commit_message>
<xml_diff>
--- a/Tutorial 1/Health Data Cluster.xlsx
+++ b/Tutorial 1/Health Data Cluster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ML\Data_Cluster_Tutorial\Tutorial 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C827E9A-83C3-41E0-B498-88340B2253FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE21586-2C12-4946-85B1-F3E2B71E340E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{55884CE1-6472-4423-86EB-4C74D723A95A}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590A7963-FDBD-4396-A6E8-0E2F13878056}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +536,7 @@
     <col min="7" max="7" width="9.36328125" customWidth="1"/>
     <col min="8" max="8" width="8.36328125" customWidth="1"/>
     <col min="9" max="9" width="7.54296875" customWidth="1"/>
-    <col min="10" max="10" width="6.1796875" customWidth="1"/>
+    <col min="10" max="10" width="8.1796875" customWidth="1"/>
     <col min="17" max="18" width="12.1796875" customWidth="1"/>
     <col min="19" max="19" width="25" customWidth="1"/>
     <col min="20" max="20" width="15.26953125" customWidth="1"/>

</xml_diff>